<commit_message>
fix opal excel error and update calculations
</commit_message>
<xml_diff>
--- a/Experiment_Planner_Stilla_dPCR_NaicaMM_Opal_Taqman.xlsx
+++ b/Experiment_Planner_Stilla_dPCR_NaicaMM_Opal_Taqman.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Genetics\13. Stilla Naica Digital PCR\Experiment Planners\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ddPCR_protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089BC1B7-3D1C-4528-9AB7-68D07B015AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13305" windowHeight="10995"/>
+    <workbookView xWindow="14100" yWindow="2535" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Conditions" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +26,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,12 +38,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>clément Gay</author>
   </authors>
   <commentList>
-    <comment ref="D13" authorId="0" shapeId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -279,7 +282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1321,14 +1324,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1616,7 @@
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
       <c r="D13" s="29">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>1</v>
@@ -1651,7 +1654,7 @@
       </c>
       <c r="D14" s="24">
         <f>C14*D13</f>
-        <v>25.6</v>
+        <v>96</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>0</v>
@@ -1689,7 +1692,7 @@
       </c>
       <c r="D15" s="21">
         <f>C15*D13</f>
-        <v>5.12</v>
+        <v>19.2</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>0</v>
@@ -1723,7 +1726,8 @@
         <v>0.64</v>
       </c>
       <c r="D16" s="62">
-        <v>40</v>
+        <f>C16*D13</f>
+        <v>38.4</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>42</v>
@@ -1781,7 +1785,7 @@
       </c>
       <c r="D18" s="63">
         <f>D19-D14-D15-D16</f>
-        <v>41.28</v>
+        <v>266.40000000000003</v>
       </c>
       <c r="E18" s="60"/>
       <c r="I18" s="80"/>
@@ -1808,7 +1812,7 @@
       </c>
       <c r="D19" s="26">
         <f>D13*7</f>
-        <v>112</v>
+        <v>420</v>
       </c>
       <c r="I19" s="80"/>
       <c r="J19" s="83"/>

</xml_diff>